<commit_message>
moved write deck to own file
</commit_message>
<xml_diff>
--- a/Project/Data/rand_deck_1.xlsx
+++ b/Project/Data/rand_deck_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>score</t>
+          <t>iscommander</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -454,6 +454,31 @@
           <t>mana_cost</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>isramp</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ramp_value</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>isdraw</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>draw_value</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>card_score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -463,12 +488,27 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -480,13 +520,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -497,13 +552,28 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -514,13 +584,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -531,13 +616,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -548,13 +648,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -565,13 +680,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -582,13 +712,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -599,12 +744,27 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -616,13 +776,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -633,13 +808,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -650,13 +840,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -667,13 +872,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -684,13 +904,28 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +936,28 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -718,13 +968,28 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -735,13 +1000,28 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -752,13 +1032,28 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -769,13 +1064,28 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -786,13 +1096,28 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
         <v>7</v>
       </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>9</v>
+      <c r="J21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -803,13 +1128,28 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>7</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -820,13 +1160,28 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="24">
@@ -837,12 +1192,27 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
       </c>
       <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -854,13 +1224,28 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
         <v>7</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -871,13 +1256,28 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -888,13 +1288,28 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -905,13 +1320,28 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -922,13 +1352,28 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -939,13 +1384,28 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -956,12 +1416,27 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -973,13 +1448,28 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -990,13 +1480,28 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>6</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1007,13 +1512,28 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1024,13 +1544,28 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
         <v>2</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1041,12 +1576,27 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1058,12 +1608,27 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1075,13 +1640,28 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1092,13 +1672,28 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1109,13 +1704,28 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
+        <v>6</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
         <v>2</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>3</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1126,12 +1736,27 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1143,12 +1768,27 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
       </c>
       <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1160,13 +1800,28 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1177,13 +1832,28 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1194,13 +1864,28 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>5</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1211,13 +1896,28 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
         <v>2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>7</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1228,13 +1928,28 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1245,12 +1960,27 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1262,13 +1992,28 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1279,12 +2024,27 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1296,13 +2056,28 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
         <v>5</v>
       </c>
-      <c r="D51" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" t="n">
-        <v>9</v>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1313,13 +2088,28 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1330,13 +2120,28 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1347,13 +2152,28 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1364,13 +2184,28 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1381,13 +2216,28 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1398,13 +2248,28 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1415,13 +2280,28 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
         <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1432,13 +2312,28 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
         <v>6</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>7</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1449,13 +2344,28 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1466,13 +2376,28 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1483,13 +2408,28 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1500,13 +2440,28 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="64">
@@ -1517,13 +2472,28 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1534,13 +2504,28 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
+        <v>6</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="n">
         <v>3</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1551,13 +2536,28 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
         <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1568,13 +2568,28 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1585,13 +2600,28 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1602,13 +2632,28 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
         <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1619,13 +2664,28 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1636,13 +2696,28 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -1653,13 +2728,28 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="n">
         <v>2</v>
       </c>
-      <c r="D72" t="n">
-        <v>1</v>
-      </c>
-      <c r="E72" t="n">
-        <v>8</v>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1670,13 +2760,28 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" t="n">
+        <v>2</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1687,13 +2792,28 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" t="n">
+        <v>3</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" t="n">
+        <v>3</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1704,12 +2824,27 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
       </c>
       <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1721,13 +2856,28 @@
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
+        <v>6</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1738,13 +2888,28 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
       </c>
       <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="n">
         <v>3</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" t="n">
+        <v>4</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1755,13 +2920,28 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1772,12 +2952,27 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" t="n">
+        <v>6</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1789,13 +2984,28 @@
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1806,13 +3016,28 @@
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1823,13 +3048,28 @@
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
         <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1840,13 +3080,28 @@
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
+        <v>1</v>
+      </c>
+      <c r="I83" t="n">
+        <v>7</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1857,12 +3112,27 @@
         <v>83</v>
       </c>
       <c r="C84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1874,13 +3144,28 @@
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1891,13 +3176,28 @@
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" t="n">
+        <v>1</v>
+      </c>
+      <c r="I86" t="n">
+        <v>2</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1908,13 +3208,28 @@
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1925,13 +3240,28 @@
         <v>87</v>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>1</v>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1942,13 +3272,28 @@
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90">
@@ -1959,12 +3304,27 @@
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
+        <v>7</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1976,12 +3336,27 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
       </c>
       <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1993,12 +3368,27 @@
         <v>91</v>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
+        <v>3</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2010,13 +3400,28 @@
         <v>92</v>
       </c>
       <c r="C93" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1</v>
+      </c>
+      <c r="G93" t="n">
+        <v>4</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2027,13 +3432,28 @@
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
         <v>1</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2044,13 +3464,28 @@
         <v>94</v>
       </c>
       <c r="C95" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2061,13 +3496,28 @@
         <v>95</v>
       </c>
       <c r="C96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="97">
@@ -2078,13 +3528,28 @@
         <v>96</v>
       </c>
       <c r="C97" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
         <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2095,13 +3560,28 @@
         <v>97</v>
       </c>
       <c r="C98" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
         <v>1</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2112,13 +3592,92 @@
         <v>98</v>
       </c>
       <c r="C99" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>99</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>100</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>